<commit_message>
Working on RT quantile of Model Preds
</commit_message>
<xml_diff>
--- a/models/code/criterionVar/Criterionx/groupFits.xlsx
+++ b/models/code/criterionVar/Criterionx/groupFits.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16725" windowHeight="11100" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16725" windowHeight="11100"/>
   </bookViews>
   <sheets>
     <sheet name="Mix" sheetId="1" r:id="rId1"/>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,6 +645,94 @@
         <v>0.752632464327746</v>
       </c>
     </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>25407.294767783998</v>
+      </c>
+      <c r="B7">
+        <v>50921.243024738302</v>
+      </c>
+      <c r="C7">
+        <v>2.8481542798030102</v>
+      </c>
+      <c r="D7">
+        <v>-2.1456130861643402E-3</v>
+      </c>
+      <c r="E7">
+        <v>3.0449411611117898</v>
+      </c>
+      <c r="F7">
+        <v>-5.9347709033486201E-4</v>
+      </c>
+      <c r="G7">
+        <v>1.37083179388561E-2</v>
+      </c>
+      <c r="H7">
+        <v>1.7523330350945499E-2</v>
+      </c>
+      <c r="I7">
+        <v>2.5827938831575601</v>
+      </c>
+      <c r="J7">
+        <v>1.37636969257252</v>
+      </c>
+      <c r="K7">
+        <v>0.53153711445798002</v>
+      </c>
+      <c r="L7">
+        <v>0.55957907482013203</v>
+      </c>
+      <c r="M7">
+        <v>1.6700002437178899E-2</v>
+      </c>
+      <c r="N7">
+        <v>1.18336697194636</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>12704.991302479</v>
+      </c>
+      <c r="B8">
+        <v>25515.620089727901</v>
+      </c>
+      <c r="C8">
+        <v>2.6604749466414002</v>
+      </c>
+      <c r="D8">
+        <v>-2.7833118585753802E-3</v>
+      </c>
+      <c r="E8">
+        <v>2.6355004374362498</v>
+      </c>
+      <c r="F8">
+        <v>1.2307569401619299E-2</v>
+      </c>
+      <c r="G8">
+        <v>7.2504124725386102E-3</v>
+      </c>
+      <c r="H8">
+        <v>2.41637765593459E-3</v>
+      </c>
+      <c r="I8">
+        <v>2.4595685060864301</v>
+      </c>
+      <c r="J8">
+        <v>1.3843859672882599</v>
+      </c>
+      <c r="K8">
+        <v>0.57530656722347095</v>
+      </c>
+      <c r="L8">
+        <v>0.61887395687995705</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2.74082775257352E-5</v>
+      </c>
+      <c r="N8">
+        <v>1.2116137146980599</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -652,10 +740,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,6 +939,76 @@
         <v>2.2982104797751499</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>23810.334830759999</v>
+      </c>
+      <c r="B7">
+        <v>47700.659778397698</v>
+      </c>
+      <c r="C7">
+        <v>1.8581938519516501</v>
+      </c>
+      <c r="D7">
+        <v>1.09097621350335E-2</v>
+      </c>
+      <c r="E7">
+        <v>1.5631309781263201</v>
+      </c>
+      <c r="F7">
+        <v>0.69289979756507702</v>
+      </c>
+      <c r="G7">
+        <v>1.1299878145219999</v>
+      </c>
+      <c r="H7">
+        <v>2.0861571160376599E-3</v>
+      </c>
+      <c r="I7">
+        <v>1.46244802337094</v>
+      </c>
+      <c r="J7">
+        <v>0.62409911007868701</v>
+      </c>
+      <c r="K7">
+        <v>1.87993837822989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13784.9478595788</v>
+      </c>
+      <c r="B8">
+        <v>27649.123832735</v>
+      </c>
+      <c r="C8">
+        <v>1.8581938519516501</v>
+      </c>
+      <c r="D8">
+        <v>1.09097621350335E-2</v>
+      </c>
+      <c r="E8">
+        <v>1.5631309781263201</v>
+      </c>
+      <c r="F8">
+        <v>0.69289979756507702</v>
+      </c>
+      <c r="G8">
+        <v>1.1299878145219999</v>
+      </c>
+      <c r="H8">
+        <v>2.0861571160376599E-3</v>
+      </c>
+      <c r="I8">
+        <v>1.46244802337094</v>
+      </c>
+      <c r="J8">
+        <v>0.62409911007868701</v>
+      </c>
+      <c r="K8">
+        <v>1.87993837822989</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>